<commit_message>
Added and normalize codes + document drag'n'drop and planification
</commit_message>
<xml_diff>
--- a/Documentation/PlanningActuel.xlsx
+++ b/Documentation/PlanningActuel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7624695b9c6b502a/Scrum-o-Wall/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7624695b9c6b502a/Scrum-o-Wall/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="260" documentId="11_AD4D9D64A577C15A4A541898F85C516A5BDEDD82" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B420EFE2-CB87-4A3F-AFD8-F6FBDB243652}"/>
+  <xr:revisionPtr revIDLastSave="302" documentId="11_AD4D9D64A577C15A4A541898F85C516A5BDEDD82" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EA6D71E8-C5BB-4BE0-97B0-66F39DC83CE9}"/>
   <bookViews>
-    <workbookView xWindow="3585" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>Planning du travail de diplôme</t>
   </si>
@@ -117,6 +117,12 @@
   </si>
   <si>
     <t>Jalon</t>
+  </si>
+  <si>
+    <t>Création de fenêtres pop-up</t>
+  </si>
+  <si>
+    <t>Tests unitaires</t>
   </si>
 </sst>
 </file>
@@ -668,10 +674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -719,7 +725,7 @@
         <v>18</v>
       </c>
       <c r="D3" s="12">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E3" s="13"/>
     </row>
@@ -734,7 +740,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="4">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="E4" s="7"/>
     </row>
@@ -749,7 +755,7 @@
         <v>0.5</v>
       </c>
       <c r="D5" s="4">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E5" s="7"/>
     </row>
@@ -779,7 +785,7 @@
         <v>3</v>
       </c>
       <c r="D7" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7" s="7"/>
     </row>
@@ -794,7 +800,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="4">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="E8" s="7"/>
     </row>
@@ -808,7 +814,9 @@
       <c r="C9" s="4">
         <v>1</v>
       </c>
-      <c r="D9" s="4"/>
+      <c r="D9" s="4">
+        <v>1</v>
+      </c>
       <c r="E9" s="7"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -821,7 +829,9 @@
       <c r="C10" s="4">
         <v>1</v>
       </c>
-      <c r="D10" s="4"/>
+      <c r="D10" s="4">
+        <v>1</v>
+      </c>
       <c r="E10" s="7"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -835,7 +845,7 @@
         <v>3</v>
       </c>
       <c r="D11" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" s="7"/>
     </row>
@@ -850,7 +860,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="4">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E12" s="7"/>
     </row>
@@ -864,7 +874,9 @@
       <c r="C13" s="4">
         <v>1</v>
       </c>
-      <c r="D13" s="4"/>
+      <c r="D13" s="4">
+        <v>1</v>
+      </c>
       <c r="E13" s="7"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -877,7 +889,9 @@
       <c r="C14" s="4">
         <v>1</v>
       </c>
-      <c r="D14" s="4"/>
+      <c r="D14" s="4">
+        <v>1</v>
+      </c>
       <c r="E14" s="7"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -905,7 +919,9 @@
       <c r="C16" s="4">
         <v>2</v>
       </c>
-      <c r="D16" s="4"/>
+      <c r="D16" s="4">
+        <v>3</v>
+      </c>
       <c r="E16" s="6"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -918,46 +934,48 @@
       <c r="C17" s="4">
         <v>2</v>
       </c>
-      <c r="D17" s="4"/>
+      <c r="D17" s="4">
+        <v>0</v>
+      </c>
       <c r="E17" s="6"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>27</v>
+      <c r="A18" s="5">
+        <v>16</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="6">
-        <v>43945</v>
-      </c>
+      <c r="D18" s="4">
+        <v>3</v>
+      </c>
+      <c r="E18" s="6"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>27</v>
+      <c r="A19" s="5">
+        <v>17</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="6">
-        <v>43958</v>
-      </c>
+      <c r="D19" s="4">
+        <v>3</v>
+      </c>
+      <c r="E19" s="6"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="6">
-        <v>43959</v>
+        <v>43945</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -965,12 +983,12 @@
         <v>27</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="6">
-        <v>43966</v>
+        <v>43958</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -978,25 +996,57 @@
         <v>27</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="6">
+        <v>43959</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="6">
+        <v>43966</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="6">
         <v>43973</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="8" t="s">
+    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B25" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="10">
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="10">
         <v>43990</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <f>SUM(D3:D25)</f>
+        <v>38.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>